<commit_message>
Version 5 : Separating action keywords and object using OR file
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -79,9 +79,6 @@
     <t>navigateUrl</t>
   </si>
   <si>
-    <t>clickButton</t>
-  </si>
-  <si>
     <t>waitSometime</t>
   </si>
   <si>
@@ -92,6 +89,21 @@
   </si>
   <si>
     <t>input_upass</t>
+  </si>
+  <si>
+    <t>txt_name</t>
+  </si>
+  <si>
+    <t>txt_pass</t>
+  </si>
+  <si>
+    <t>btn_login</t>
+  </si>
+  <si>
+    <t>Page_Object</t>
+  </si>
+  <si>
+    <t>click</t>
   </si>
 </sst>
 </file>
@@ -449,21 +461,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="3" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,10 +486,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -487,11 +502,12 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -501,11 +517,12 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -516,10 +533,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -530,10 +550,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -544,10 +567,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -557,11 +583,12 @@
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -571,8 +598,9 @@
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 6 : Test Suite
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -104,6 +105,24 @@
   </si>
   <si>
     <t>click</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Login to the Salesforce</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TS008</t>
   </si>
 </sst>
 </file>
@@ -154,9 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +623,75 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 7 : Log Files added
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -117,12 +117,6 @@
   </si>
   <si>
     <t>TC002</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TS008</t>
   </si>
 </sst>
 </file>
@@ -481,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,16 +622,110 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -649,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +777,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 8 : Test Reports
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="6060" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="6060" windowWidth="15705" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
+    <sheet name="Test Cases" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -117,12 +117,19 @@
   </si>
   <si>
     <t>TC002</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,18 +172,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -193,10 +200,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -231,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,7 +273,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,7 +361,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -363,13 +370,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -379,7 +386,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -388,7 +395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -397,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -407,12 +414,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -443,7 +450,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -462,7 +469,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -474,22 +481,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F2" sqref="F2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +512,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -520,8 +530,11 @@
       <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -535,8 +548,11 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -552,8 +568,11 @@
       <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -569,8 +588,11 @@
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -586,8 +608,11 @@
       <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -601,8 +626,11 @@
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,8 +644,11 @@
       <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -631,8 +662,11 @@
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -646,8 +680,11 @@
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -663,8 +700,11 @@
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -680,8 +720,11 @@
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -697,8 +740,11 @@
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -712,8 +758,11 @@
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -727,27 +776,30 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="62.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,8 +809,11 @@
       <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -768,8 +823,11 @@
       <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -779,8 +837,11 @@
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 9 : Adding Data Set (Data Drivern)
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -86,12 +86,6 @@
     <t>closeBrowser</t>
   </si>
   <si>
-    <t>input_uname</t>
-  </si>
-  <si>
-    <t>input_upass</t>
-  </si>
-  <si>
     <t>txt_name</t>
   </si>
   <si>
@@ -120,6 +114,21 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Data_Set</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>rajasingh.nadar@infosys.com.vmstdemo</t>
+  </si>
+  <si>
+    <t>Raja@1506$$$$$$</t>
   </si>
   <si>
     <t>PASS</t>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,9 +503,10 @@
     <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
     <col min="3" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="38.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,16 +517,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -531,10 +544,13 @@
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -548,11 +564,12 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,16 +580,19 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,16 +603,19 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -603,16 +626,17 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -626,11 +650,12 @@
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,13 +669,14 @@
       <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -663,12 +689,15 @@
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -680,13 +709,14 @@
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -695,18 +725,21 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -715,18 +748,21 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -735,18 +771,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
@@ -758,13 +795,14 @@
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
@@ -776,8 +814,9 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>35</v>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +829,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,10 +846,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,27 +857,27 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 10 : Final version with comments
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6060" windowWidth="15705" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="6060"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
-    <sheet name="Test Cases" r:id="rId2" sheetId="2"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -138,7 +138,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,18 +180,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -209,10 +208,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -247,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,7 +281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,7 +369,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -379,13 +378,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -395,7 +394,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -404,7 +403,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -413,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -423,12 +422,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -459,7 +458,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -478,7 +477,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -490,20 +489,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="38.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -820,22 +819,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="62.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,6 +880,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 11 : GitHub and Jenkins execution
</commit_message>
<xml_diff>
--- a/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDrivernFrameWork/src/dataEngine/DataEngine.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="6060"/>
+    <workbookView windowHeight="6060" windowWidth="15705" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Steps" r:id="rId1" sheetId="1"/>
+    <sheet name="Test Cases" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:F18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="39">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -138,6 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,18 +182,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -208,10 +210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -246,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,7 +371,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -378,13 +380,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -394,7 +396,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -403,7 +405,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -412,7 +414,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -422,12 +424,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -458,7 +460,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -477,7 +479,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -489,20 +491,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="38.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,22 +821,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="62.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="62.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,6 +882,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>